<commit_message>
add content to bootstrap
</commit_message>
<xml_diff>
--- a/bootstrap.xlsx
+++ b/bootstrap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t xml:space="preserve">&lt;!DOCTYPE html&gt;
 &lt;html&gt;
@@ -308,6 +308,489 @@
   <si>
     <t>button w .btn</t>
   </si>
+  <si>
+    <t>Nesting Button Groups &amp; Dropdown Menus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;div class="container"&gt;
+  &lt;h2&gt;Nesting Button Groups&lt;/h2&gt;
+  &lt;p&gt;Nest button groups to create drop down menus:&lt;/p&gt;
+  &lt;div class="btn-group"&gt;
+    &lt;button type="button" class="btn btn-primary"&gt;Apple&lt;/button&gt;
+    &lt;button type="button" class="btn btn-primary"&gt;Samsung&lt;/button&gt;
+    &lt;div class="btn-group"&gt;
+      &lt;button type="button" class="btn btn-primary dropdown-toggle" data-toggle="dropdown"&gt;
+      Sony &lt;span class="caret"&gt;&lt;/span&gt;&lt;/button&gt;
+      &lt;ul class="dropdown-menu" role="menu"&gt;
+        &lt;li&gt;&lt;a href="#"&gt;Tablet&lt;/a&gt;&lt;/li&gt;
+        &lt;li&gt;&lt;a href="#"&gt;Smartphone&lt;/a&gt;&lt;/li&gt;
+      &lt;/ul&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Badges</t>
+  </si>
+  <si>
+    <t>&lt;a href="#"&gt;News &lt;span class="badge"&gt;5&lt;/span&gt;&lt;/a&gt;&lt;br&gt;
+&lt;a href="#"&gt;Comments &lt;span class="badge"&gt;10&lt;/span&gt;&lt;/a&gt;&lt;br&gt;
+&lt;a href="#"&gt;Updates &lt;span class="badge"&gt;2&lt;/span&gt;&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;Example &lt;span class="label label-default"&gt;New&lt;/span&gt;&lt;/h1&gt;
+&lt;h2&gt;Example &lt;span class="label label-default"&gt;New&lt;/span&gt;&lt;/h2&gt;
+&lt;h3&gt;Example &lt;span class="label label-default"&gt;New&lt;/span&gt;&lt;/h3&gt;
+&lt;h4&gt;Example &lt;span class="label label-default"&gt;New&lt;/span&gt;&lt;/h4&gt;
+&lt;h5&gt;Example &lt;span class="label label-default"&gt;New&lt;/span&gt;&lt;/h5&gt;
+&lt;h6&gt;Example &lt;span class="label label-default"&gt;New&lt;/span&gt;&lt;/h6&gt;
+&lt;span class="label label-default"&gt;Default Label&lt;/span&gt;
+&lt;span class="label label-primary"&gt;Primary Label&lt;/span&gt;
+&lt;span class="label label-success"&gt;Success Label&lt;/span&gt;
+&lt;span class="label label-info"&gt;Info Label&lt;/span&gt;
+&lt;span class="label label-warning"&gt;Warning Label&lt;/span&gt;
+&lt;span class="label label-danger"&gt;Danger Label&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Striped Progress Bars</t>
+  </si>
+  <si>
+    <t>&lt;div class="progress"&gt;
+  &lt;div class="progress-bar progress-bar-success progress-bar-striped" role="progressbar"
+  aria-valuenow="40" aria-valuemin="0" aria-valuemax="100" style="width:40%"&gt;
+    40% Complete (success)
+  &lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="progress"&gt;
+  &lt;div class="progress-bar progress-bar-info progress-bar-striped" role="progressbar"
+  aria-valuenow="50" aria-valuemin="0" aria-valuemax="100" style="width:50%"&gt;
+    50% Complete (info)
+  &lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="progress"&gt;
+  &lt;div class="progress-bar progress-bar-warning progress-bar-striped" role="progressbar"
+  aria-valuenow="60" aria-valuemin="0" aria-valuemax="100" style="width:60%"&gt;
+    60% Complete (warning)
+  &lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="progress"&gt;
+  &lt;div class="progress-bar progress-bar-danger progress-bar-striped" role="progressbar"
+  aria-valuenow="70" aria-valuemin="0" aria-valuemax="100" style="width:70%"&gt;
+    70% Complete (danger)
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Animated Progress Bar</t>
+  </si>
+  <si>
+    <t>&lt;div class="progress"&gt;
+  &lt;div class="progress-bar progress-bar-striped active" role="progressbar"
+  aria-valuenow="40" aria-valuemin="0" aria-valuemax="100" style="width:40%"&gt;
+    40%
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Pagination w Active State</t>
+  </si>
+  <si>
+    <t>&lt;ul class="pagination"&gt;
+  &lt;li&gt;&lt;a href="#"&gt;1&lt;/a&gt;&lt;/li&gt;
+  &lt;li class="active"&gt;&lt;a href="#"&gt;2&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;3&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;4&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;5&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Pager</t>
+  </si>
+  <si>
+    <t>&lt;ul class="pager"&gt;
+  &lt;li class="previous"&gt;&lt;a href="#"&gt;Previous&lt;/a&gt;&lt;/li&gt;
+  &lt;li class="next"&gt;&lt;a href="#"&gt;Next&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Basic List Groups</t>
+  </si>
+  <si>
+    <t>&lt;ul class="list-group"&gt;
+  &lt;li class="list-group-item"&gt;First item&lt;/li&gt;
+  &lt;li class="list-group-item"&gt;Second item&lt;/li&gt;
+  &lt;li class="list-group-item"&gt;Third item&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Panels</t>
+  </si>
+  <si>
+    <t>&lt;div class="panel panel-default"&gt;
+ &lt;div class="panel-heading"&gt;Panel Heading&lt;/div&gt;
+  &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+  &lt;div class="panel-footer"&gt;Panel Footer&lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Panels with Contextual Classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;div class="container"&gt;
+  &lt;h2&gt;Panels with Contextual Classes&lt;/h2&gt;
+  &lt;div class="panel-group"&gt;
+    &lt;div class="panel panel-default"&gt;
+      &lt;div class="panel-heading"&gt;Panel with panel-default class&lt;/div&gt;
+      &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+    &lt;/div&gt;
+    &lt;div class="panel panel-primary"&gt;
+      &lt;div class="panel-heading"&gt;Panel with panel-primary class&lt;/div&gt;
+      &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+    &lt;/div&gt;
+    &lt;div class="panel panel-success"&gt;
+      &lt;div class="panel-heading"&gt;Panel with panel-success class&lt;/div&gt;
+      &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+    &lt;/div&gt;
+    &lt;div class="panel panel-info"&gt;
+      &lt;div class="panel-heading"&gt;Panel with panel-info class&lt;/div&gt;
+      &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+    &lt;/div&gt;
+    &lt;div class="panel panel-warning"&gt;
+      &lt;div class="panel-heading"&gt;Panel with panel-warning class&lt;/div&gt;
+      &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+    &lt;/div&gt;
+    &lt;div class="panel panel-danger"&gt;
+      &lt;div class="panel-heading"&gt;Panel with panel-danger class&lt;/div&gt;
+      &lt;div class="panel-body"&gt;Panel Content&lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;div class="container"&gt;
+  &lt;h2&gt;Dropdowns&lt;/h2&gt;
+  &lt;p&gt;The .dropdown-header class is used to add headers inside the dropdown menu:&lt;/p&gt;
+  &lt;div class="dropdown"&gt;
+    &lt;button class="btn btn-default dropdown-toggle" type="button" data-toggle="dropdown"&gt;Tutorials
+    &lt;span class="caret"&gt;&lt;/span&gt;&lt;/button&gt;
+    &lt;ul class="dropdown-menu"&gt;
+      &lt;li class="dropdown-header"&gt;Dropdown header 1&lt;/li&gt;
+      &lt;li&gt;&lt;a href="#"&gt;HTML&lt;/a&gt;&lt;/li&gt;
+      &lt;li&gt;&lt;a href="#"&gt;CSS&lt;/a&gt;&lt;/li&gt;
+      &lt;li&gt;&lt;a href="#"&gt;JavaScript&lt;/a&gt;&lt;/li&gt;
+      &lt;li class="divider"&gt;&lt;/li&gt;
+      &lt;li class="dropdown-header"&gt;Dropdown header 2&lt;/li&gt;
+      &lt;li&gt;&lt;a href="#"&gt;About Us&lt;/a&gt;&lt;/li&gt;
+    &lt;/ul&gt;
+  &lt;/div&gt;
+&lt;/div&gt;
+</t>
+  </si>
+  <si>
+    <t>Accordion (Collopse Panel)</t>
+  </si>
+  <si>
+    <t>&lt;div class="panel-group" id="accordion"&gt;
+  &lt;div class="panel panel-default"&gt;
+    &lt;div class="panel-heading"&gt;
+      &lt;h4 class="panel-title"&gt;
+        &lt;a data-toggle="collapse" data-parent="#accordion" href="#collapse1"&gt;
+        Collapsible Group 1&lt;/a&gt;
+      &lt;/h4&gt;
+    &lt;/div&gt;
+    &lt;div id="collapse1" class="panel-collapse collapse in"&gt;
+      &lt;div class="panel-body"&gt;Lorem ipsum dolor sit amet, consectetur adipisicing elit,
+      sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad
+      minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea
+      commodo consequat.&lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div class="panel panel-default"&gt;
+    &lt;div class="panel-heading"&gt;
+      &lt;h4 class="panel-title"&gt;
+        &lt;a data-toggle="collapse" data-parent="#accordion" href="#collapse2"&gt;
+        Collapsible Group 2&lt;/a&gt;
+      &lt;/h4&gt;
+    &lt;/div&gt;
+    &lt;div id="collapse2" class="panel-collapse collapse"&gt;
+      &lt;div class="panel-body"&gt;Lorem ipsum dolor sit amet, consectetur adipisicing elit,
+      sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad
+      minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea
+      commodo consequat.&lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div class="panel panel-default"&gt;
+    &lt;div class="panel-heading"&gt;
+      &lt;h4 class="panel-title"&gt;
+        &lt;a data-toggle="collapse" data-parent="#accordion" href="#collapse3"&gt;
+        Collapsible Group 3&lt;/a&gt;
+      &lt;/h4&gt;
+    &lt;/div&gt;
+    &lt;div id="collapse3" class="panel-collapse collapse"&gt;
+      &lt;div class="panel-body"&gt;Lorem ipsum dolor sit amet, consectetur adipisicing elit,
+      sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad
+      minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea
+      commodo consequat.&lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Menus</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Home&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 1&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 2&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 3&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Tabs</t>
+  </si>
+  <si>
+    <t>&lt;ul class="nav nav-tabs"&gt;
+  &lt;li class="active"&gt;&lt;a href="#"&gt;Home&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 1&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 2&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 3&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Pills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul class="nav nav-pills"&gt;
+  &lt;li class="active"&gt;&lt;a href="#"&gt;Home&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 1&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 2&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 3&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Centered Tabs and Pills</t>
+  </si>
+  <si>
+    <t>&lt;!-- Centered Tabs --&gt;
+&lt;ul class="nav nav-tabs nav-justified"&gt;
+  &lt;li class="active"&gt;&lt;a href="#"&gt;Home&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 1&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 2&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 3&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;!-- Centered Pills --&gt;
+&lt;ul class="nav nav-pills nav-justified"&gt;
+  &lt;li class="active"&gt;&lt;a href="#"&gt;Home&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 1&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 2&lt;/a&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;a href="#"&gt;Menu 3&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Collapsing The Navigation Bar</t>
+  </si>
+  <si>
+    <t>&lt;nav class="navbar navbar-inverse"&gt;
+  &lt;div class="container-fluid"&gt;
+    &lt;div class="navbar-header"&gt;
+      &lt;button type="button" class="navbar-toggle" data-toggle="collapse" data-target="#myNavbar"&gt;
+        &lt;span class="icon-bar"&gt;&lt;/span&gt;
+        &lt;span class="icon-bar"&gt;&lt;/span&gt;
+        &lt;span class="icon-bar"&gt;&lt;/span&gt; 
+      &lt;/button&gt;
+      &lt;a class="navbar-brand" href="#"&gt;WebSiteName&lt;/a&gt;
+    &lt;/div&gt;
+    &lt;div class="collapse navbar-collapse" id="myNavbar"&gt;
+      &lt;ul class="nav navbar-nav"&gt;
+        &lt;li class="active"&gt;&lt;a href="#"&gt;Home&lt;/a&gt;&lt;/li&gt;
+        &lt;li&gt;&lt;a href="#"&gt;Page 1&lt;/a&gt;&lt;/li&gt;
+        &lt;li&gt;&lt;a href="#"&gt;Page 2&lt;/a&gt;&lt;/li&gt; 
+        &lt;li&gt;&lt;a href="#"&gt;Page 3&lt;/a&gt;&lt;/li&gt; 
+      &lt;/ul&gt;
+      &lt;ul class="nav navbar-nav navbar-right"&gt;
+        &lt;li&gt;&lt;a href="#"&gt;&lt;span class="glyphicon glyphicon-user"&gt;&lt;/span&gt; Sign Up&lt;/a&gt;&lt;/li&gt;
+        &lt;li&gt;&lt;a href="#"&gt;&lt;span class="glyphicon glyphicon-log-in"&gt;&lt;/span&gt; Login&lt;/a&gt;&lt;/li&gt;
+      &lt;/ul&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/nav&gt;</t>
+  </si>
+  <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>&lt;form role="form"&gt;
+  &lt;div class="form-group"&gt;
+    &lt;label for="email"&gt;Email address:&lt;/label&gt;
+    &lt;input type="email" class="form-control" id="email"&gt;
+  &lt;/div&gt;
+  &lt;div class="form-group"&gt;
+    &lt;label for="pwd"&gt;Password:&lt;/label&gt;
+    &lt;input type="password" class="form-control" id="pwd"&gt;
+  &lt;/div&gt;
+  &lt;div class="checkbox"&gt;
+    &lt;label&gt;&lt;input type="checkbox"&gt; Remember me&lt;/label&gt;
+  &lt;/div&gt;
+  &lt;button type="submit" class="btn btn-default"&gt;Submit&lt;/button&gt;
+&lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>Horizontal Form</t>
+  </si>
+  <si>
+    <t>&lt;form class="form-horizontal" role="form"&gt;
+  &lt;div class="form-group"&gt;
+    &lt;label class="control-label col-sm-2" for="email"&gt;Email:&lt;/label&gt;
+    &lt;div class="col-sm-10"&gt;
+      &lt;input type="email" class="form-control" id="email" placeholder="Enter email"&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div class="form-group"&gt;
+    &lt;label class="control-label col-sm-2" for="pwd"&gt;Password:&lt;/label&gt;
+    &lt;div class="col-sm-10"&gt; 
+      &lt;input type="password" class="form-control" id="pwd" placeholder="Enter password"&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div class="form-group"&gt; 
+    &lt;div class="col-sm-offset-2 col-sm-10"&gt;
+      &lt;div class="checkbox"&gt;
+        &lt;label&gt;&lt;input type="checkbox"&gt; Remember me&lt;/label&gt;
+      &lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;div class="form-group"&gt; 
+    &lt;div class="col-sm-offset-2 col-sm-10"&gt;
+      &lt;button type="submit" class="btn btn-default"&gt;Submit&lt;/button&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Textarea</t>
+  </si>
+  <si>
+    <t>Checkboxes</t>
+  </si>
+  <si>
+    <t>Radio Buttons</t>
+  </si>
+  <si>
+    <t>Select List</t>
+  </si>
+  <si>
+    <t>&lt;div class="form-group"&gt;
+  &lt;label for="sel1"&gt;Select list:&lt;/label&gt;
+  &lt;select class="form-control" id="sel1"&gt;
+    &lt;option&gt;1&lt;/option&gt;
+    &lt;option&gt;2&lt;/option&gt;
+    &lt;option&gt;3&lt;/option&gt;
+    &lt;option&gt;4&lt;/option&gt;
+  &lt;/select&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;label class="radio-inline"&gt;&lt;input type="radio" name="optradio"&gt;Option 1&lt;/label&gt;
+&lt;label class="radio-inline"&gt;&lt;input type="radio" name="optradio"&gt;Option 2&lt;/label&gt;
+&lt;label class="radio-inline"&gt;&lt;input type="radio" name="optradio"&gt;Option 3&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;label class="checkbox-inline"&gt;&lt;input type="checkbox" value=""&gt;Option 1&lt;/label&gt;
+&lt;label class="checkbox-inline"&gt;&lt;input type="checkbox" value=""&gt;Option 2&lt;/label&gt;
+&lt;label class="checkbox-inline"&gt;&lt;input type="checkbox" value=""&gt;Option 3&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="form-group"&gt;
+  &lt;label for="comment"&gt;Comment:&lt;/label&gt;
+  &lt;textarea class="form-control" rows="5" id="comment"&gt;&lt;/textarea&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="form-group"&gt;
+  &lt;label for="usr"&gt;Name:&lt;/label&gt;
+  &lt;input type="text" class="form-control" id="usr"&gt;
+&lt;/div&gt;
+&lt;div class="form-group"&gt;
+  &lt;label for="pwd"&gt;Password:&lt;/label&gt;
+  &lt;input type="password" class="form-control" id="pwd"&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div id="myCarousel" class="carousel slide" data-ride="carousel"&gt;
+  &lt;!-- Indicators --&gt;
+  &lt;ol class="carousel-indicators"&gt;
+    &lt;li data-target="#myCarousel" data-slide-to="0" class="active"&gt;&lt;/li&gt;
+    &lt;li data-target="#myCarousel" data-slide-to="1"&gt;&lt;/li&gt;
+    &lt;li data-target="#myCarousel" data-slide-to="2"&gt;&lt;/li&gt;
+    &lt;li data-target="#myCarousel" data-slide-to="3"&gt;&lt;/li&gt;
+  &lt;/ol&gt;
+  &lt;!-- Wrapper for slides --&gt;
+  &lt;div class="carousel-inner" role="listbox"&gt;
+    &lt;div class="item active"&gt;
+      &lt;img src="img_chania.jpg" alt="Chania"&gt;
+    &lt;/div&gt;
+    &lt;div class="item"&gt;
+      &lt;img src="img_chania2.jpg" alt="Chania"&gt;
+    &lt;/div&gt;
+    &lt;div class="item"&gt;
+      &lt;img src="img_flower.jpg" alt="Flower"&gt;
+    &lt;/div&gt;
+    &lt;div class="item"&gt;
+      &lt;img src="img_flower2.jpg" alt="Flower"&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+  &lt;!-- Left and right controls --&gt;
+  &lt;a class="left carousel-control" href="#myCarousel" role="button" data-slide="prev"&gt;
+    &lt;span class="glyphicon glyphicon-chevron-left" aria-hidden="true"&gt;&lt;/span&gt;
+    &lt;span class="sr-only"&gt;Previous&lt;/span&gt;
+  &lt;/a&gt;
+  &lt;a class="right carousel-control" href="#myCarousel" role="button" data-slide="next"&gt;
+    &lt;span class="glyphicon glyphicon-chevron-right" aria-hidden="true"&gt;&lt;/span&gt;
+    &lt;span class="sr-only"&gt;Next&lt;/span&gt;
+  &lt;/a&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Carousel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modal </t>
+  </si>
+  <si>
+    <t>&lt;!-- Trigger the modal with a button --&gt;
+&lt;button type="button" class="btn btn-info btn-lg" data-toggle="modal" data-target="#myModal"&gt;Open Modal&lt;/button&gt;
+&lt;!-- Modal --&gt;
+&lt;div id="myModal" class="modal fade" role="dialog"&gt;
+  &lt;div class="modal-dialog"&gt;
+    &lt;!-- Modal content--&gt;
+    &lt;div class="modal-content"&gt;
+      &lt;div class="modal-header"&gt;
+        &lt;button type="button" class="close" data-dismiss="modal"&gt;&amp;times;&lt;/button&gt;
+        &lt;h4 class="modal-title"&gt;Modal Header&lt;/h4&gt;
+      &lt;/div&gt;
+      &lt;div class="modal-body"&gt;
+        &lt;p&gt;Some text in the modal.&lt;/p&gt;
+      &lt;/div&gt;
+      &lt;div class="modal-footer"&gt;
+        &lt;button type="button" class="btn btn-default" data-dismiss="modal"&gt;Close&lt;/button&gt;
+      &lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/div&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -322,12 +805,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -342,11 +831,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39" customHeight="1"/>
@@ -801,19 +1292,300 @@
       <c r="A14" t="s">
         <v>1</v>
       </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="39" customHeight="1">
       <c r="A15" t="s">
         <v>1</v>
       </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="39" customHeight="1">
       <c r="A16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="39" customHeight="1">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="39" customHeight="1">
       <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="39" customHeight="1">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="39" customHeight="1">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="39" customHeight="1">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="39" customHeight="1">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="39" customHeight="1">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="39" customHeight="1">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="39" customHeight="1">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="39" customHeight="1">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="39" customHeight="1">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="39" customHeight="1">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="39" customHeight="1">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="39" customHeight="1">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="39" customHeight="1">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="39" customHeight="1">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="39" customHeight="1">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="39" customHeight="1">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="39" customHeight="1">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="39" customHeight="1">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="39" customHeight="1">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="39" customHeight="1">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="39" customHeight="1">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="39" customHeight="1">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="39" customHeight="1">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="39" customHeight="1">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="39" customHeight="1">
+      <c r="A42" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>